<commit_message>
Bypass empty keyword cell
</commit_message>
<xml_diff>
--- a/example/tests.xlsx
+++ b/example/tests.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\robot-test-creator\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\koodi\repos\personal\robot-test-creator\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253F0782-B504-488F-AACC-184081E45039}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325BD25D-55F9-4FD3-AA8F-69EA8917E566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="2745" windowWidth="16485" windowHeight="9263" activeTab="1" xr2:uid="{7ABE35CA-173F-4660-ABC7-763F21D4B607}"/>
+    <workbookView xWindow="21285" yWindow="555" windowWidth="19170" windowHeight="15180" activeTab="2" xr2:uid="{7ABE35CA-173F-4660-ABC7-763F21D4B607}"/>
   </bookViews>
   <sheets>
     <sheet name="suite1" sheetId="1" r:id="rId1"/>
     <sheet name="suite2" sheetId="2" r:id="rId2"/>
+    <sheet name="suite3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>test case</t>
   </si>
@@ -121,8 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -141,9 +145,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -181,7 +185,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -287,7 +291,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -429,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -443,15 +447,15 @@
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,17 +469,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -483,7 +487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -491,7 +495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -502,17 +506,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -520,7 +524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -538,17 +542,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5112DA7A-B072-4FDF-A979-9E80CEEC7656}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,17 +566,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -580,7 +584,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -592,4 +596,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B238E4-E3DB-4DD2-866F-6526BAF1B930}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>